<commit_message>
Started work on an auto-level script. Probably going to abandon this in favor of one native to Foundry that builds it off of the compendium.
</commit_message>
<xml_diff>
--- a/foundryOptions.xlsx
+++ b/foundryOptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IncarnateGaming\UniversalGamingFormat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2E6CBA-DC82-432A-8D20-5108A9A8021C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9184AC8-B125-4BAA-AE24-78CB5CB9CBAE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="3195" windowWidth="15375" windowHeight="8325" xr2:uid="{D06BE2EB-E287-4F52-A712-FC8D0C089F83}"/>
+    <workbookView xWindow="26595" yWindow="1575" windowWidth="15375" windowHeight="8325" xr2:uid="{D06BE2EB-E287-4F52-A712-FC8D0C089F83}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="86">
   <si>
     <t>permission</t>
   </si>
@@ -284,6 +284,12 @@
   </si>
   <si>
     <t>Encounter</t>
+  </si>
+  <si>
+    <t>feat</t>
+  </si>
+  <si>
+    <t>class</t>
   </si>
 </sst>
 </file>
@@ -637,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685F9DF4-F257-479A-993F-E71408002C63}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,6 +921,9 @@
       <c r="G7" t="s">
         <v>16</v>
       </c>
+      <c r="I7" t="s">
+        <v>84</v>
+      </c>
       <c r="K7" t="s">
         <v>64</v>
       </c>
@@ -934,6 +943,9 @@
       </c>
       <c r="G8" t="s">
         <v>41</v>
+      </c>
+      <c r="I8" t="s">
+        <v>85</v>
       </c>
       <c r="K8" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
Version 0.0.7, August 16 2019 Alpha version.
</commit_message>
<xml_diff>
--- a/foundryOptions.xlsx
+++ b/foundryOptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IncarnateGaming\UniversalGamingFormat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9184AC8-B125-4BAA-AE24-78CB5CB9CBAE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC4C586-801B-48C2-AE66-F3B20FC1900A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26595" yWindow="1575" windowWidth="15375" windowHeight="8325" xr2:uid="{D06BE2EB-E287-4F52-A712-FC8D0C089F83}"/>
+    <workbookView xWindow="31110" yWindow="7170" windowWidth="15375" windowHeight="8325" xr2:uid="{D06BE2EB-E287-4F52-A712-FC8D0C089F83}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -651,6 +651,7 @@
   <cols>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Progress on bestiary through CR 3
</commit_message>
<xml_diff>
--- a/foundryOptions.xlsx
+++ b/foundryOptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IncarnateGaming\UniversalGamingFormat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC4C586-801B-48C2-AE66-F3B20FC1900A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205B4159-B62A-4E83-AB29-887A0D0FFFEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31110" yWindow="7170" windowWidth="15375" windowHeight="8325" xr2:uid="{D06BE2EB-E287-4F52-A712-FC8D0C089F83}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D06BE2EB-E287-4F52-A712-FC8D0C089F83}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="87">
   <si>
     <t>permission</t>
   </si>
@@ -290,6 +290,9 @@
   </si>
   <si>
     <t>class</t>
+  </si>
+  <si>
+    <t>spell</t>
   </si>
 </sst>
 </file>
@@ -643,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685F9DF4-F257-479A-993F-E71408002C63}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,6 +961,9 @@
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>27</v>
+      </c>
+      <c r="I9" t="s">
+        <v>86</v>
       </c>
       <c r="K9" t="s">
         <v>66</v>

</xml_diff>